<commit_message>
updated RegisterPage first name By locator, updated product sheet in Excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/OpenCartTestData.xlsx
+++ b/src/test/resources/testdata/OpenCartTestData.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71391376819b5ff0/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naveenautomationlabs/Documents/workspace1/March2025POMSeries/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55E3701A-C9EF-44BB-A41D-E4C4C55B43B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422DCCBC-77F6-D34C-9231-8B7C84D60B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{128C9DFC-C0CE-40FA-A831-BF7FA0B0B411}"/>
+    <workbookView xWindow="3420" yWindow="1720" windowWidth="28040" windowHeight="17440" xr2:uid="{43332C77-6133-BA4E-9F1E-234FC1B5C514}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="register" sheetId="1" r:id="rId1"/>
+    <sheet name="product" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>firstname</t>
   </si>
@@ -73,31 +85,64 @@
   </si>
   <si>
     <t>sandhya@123</t>
+  </si>
+  <si>
+    <t>7878789898</t>
+  </si>
+  <si>
+    <t>7878789890</t>
+  </si>
+  <si>
+    <t>7878789843</t>
+  </si>
+  <si>
+    <t>searchkey</t>
+  </si>
+  <si>
+    <t>productname</t>
+  </si>
+  <si>
+    <t>macbook</t>
+  </si>
+  <si>
+    <t>MacBook Pro</t>
+  </si>
+  <si>
+    <t>samsung</t>
+  </si>
+  <si>
+    <t>imac</t>
+  </si>
+  <si>
+    <t>canon</t>
+  </si>
+  <si>
+    <t>Samsung SyncMaster 941BW</t>
+  </si>
+  <si>
+    <t>iMac</t>
+  </si>
+  <si>
+    <t>Canon EOS 5D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -112,7 +157,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -142,13 +187,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -178,39 +224,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -262,7 +308,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -373,13 +419,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -388,6 +427,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -452,32 +498,53 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4E0462-9F7C-4CD6-B6B6-D4C3CFC9253A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3E9CB1-8809-7049-9A76-3A2EB0510446}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,15 +561,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
-        <v>7878789898</v>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -511,15 +578,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
-        <v>7878789890</v>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
@@ -528,15 +595,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2">
-        <v>7878789843</v>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>15</v>
@@ -547,10 +614,69 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="mailto:harpreet@123" xr:uid="{20A1FE7D-B5E7-4D93-8B75-3B92C7E9F144}"/>
-    <hyperlink ref="D3" r:id="rId2" display="mailto:ratul@123" xr:uid="{892BD5FF-3B82-43F1-8202-6C90A69C0921}"/>
-    <hyperlink ref="D4" r:id="rId3" display="mailto:sandhya@123" xr:uid="{D8EC1C85-E9B1-4F77-A5B9-2692F900A992}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{2F040C7E-64C7-A14B-9C5D-C3D45779771E}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{E2654274-C01E-124C-978E-D046582B7CCD}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{BFCB18C7-D408-3443-BA62-E71E2DDF75FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D4C459C-BCE8-064F-83B6-85272E3CFB9A}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated fixes for Regression data provider issue and product test data null issue
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/OpenCartTestData.xlsx
+++ b/src/test/resources/testdata/OpenCartTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naveenautomationlabs/Documents/workspace1/March2025POMSeries/src/test/resources/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandh\eclipse-workspace\March2025POMSeries\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422DCCBC-77F6-D34C-9231-8B7C84D60B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F004B36-39BF-4965-9A40-3826AFCDDAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="1720" windowWidth="28040" windowHeight="17440" xr2:uid="{43332C77-6133-BA4E-9F1E-234FC1B5C514}"/>
+    <workbookView xWindow="4560" yWindow="1548" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{43332C77-6133-BA4E-9F1E-234FC1B5C514}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -532,19 +521,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3E9CB1-8809-7049-9A76-3A2EB0510446}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
+    <sheetView zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.19921875" customWidth="1"/>
+    <col min="4" max="4" width="12.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -578,7 +567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -595,7 +584,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -626,17 +615,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D4C459C-BCE8-064F-83B6-85272E3CFB9A}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -644,7 +633,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -652,7 +641,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -660,7 +649,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -668,7 +657,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>

</xml_diff>